<commit_message>
Push selenium maven framwork
</commit_message>
<xml_diff>
--- a/SeleniumMavenFrameworkWithJava/src/test/java/excelUtils/LoginData.xlsx
+++ b/SeleniumMavenFrameworkWithJava/src/test/java/excelUtils/LoginData.xlsx
@@ -8,17 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHANDRASEKHARJANGA\git\SeleniumPOC\SeleniumMavenFrameworkWithJava\src\test\java\excelUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD62D423-0102-4EBD-8EC1-210E42914F1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA90FA57-295C-4871-A3E7-FF0CBECCEFE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginSheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -386,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
@@ -399,19 +405,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>